<commit_message>
Add sample site and fourm tests
</commit_message>
<xml_diff>
--- a/Robot_tests/testdata_excel.xlsx
+++ b/Robot_tests/testdata_excel.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BrodyE\QACommunity\Robot_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC487A22-BDC7-4BBB-8558-05C3EE21A935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A793BB34-A882-4C90-B0E4-E7291AAF7E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{94F194FB-F599-4E1C-9BEA-12EF5846CDD9}"/>
   </bookViews>
   <sheets>
-    <sheet name="testdata" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -922,7 +922,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>